<commit_message>
fixed dingtalk report style and sheet_filelds
</commit_message>
<xml_diff>
--- a/cases/cases/test_cases.xlsx
+++ b/cases/cases/test_cases.xlsx
@@ -2122,8 +2122,8 @@
   </sheetPr>
   <dimension ref="A1:AA7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="U7" sqref="U7"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="25.7777777777778" defaultRowHeight="50" customHeight="1" outlineLevelRow="6" outlineLevelCol="0"/>
@@ -2134,19 +2134,19 @@
     <col width="4.27407407407407" customWidth="1" style="3" min="4" max="4"/>
     <col width="5.27407407407407" customWidth="1" style="3" min="5" max="5"/>
     <col width="7.91111111111111" customWidth="1" style="3" min="6" max="6"/>
-    <col width="29.9851851851852" customWidth="1" style="10" min="7" max="7"/>
+    <col width="16.6592592592593" customWidth="1" style="10" min="7" max="7"/>
     <col width="20.1851851851852" customWidth="1" style="3" min="8" max="8"/>
-    <col width="14.7259259259259" customWidth="1" style="3" min="9" max="9"/>
+    <col width="14.1185185185185" customWidth="1" style="3" min="9" max="9"/>
     <col width="9.18518518518519" customWidth="1" style="3" min="10" max="10"/>
     <col width="19.7259259259259" customWidth="1" style="10" min="11" max="11"/>
     <col width="14.637037037037" customWidth="1" style="3" min="12" max="12"/>
-    <col width="39.4296296296296" customWidth="1" style="3" min="13" max="13"/>
+    <col width="15.237037037037" customWidth="1" style="3" min="13" max="13"/>
     <col width="19.5481481481481" customWidth="1" style="3" min="14" max="14"/>
     <col width="19.8148148148148" customWidth="1" style="3" min="15" max="15"/>
-    <col width="14.2740740740741" customWidth="1" style="3" min="16" max="16"/>
+    <col width="10.1481481481481" customWidth="1" style="3" min="16" max="16"/>
     <col width="6.36296296296296" customWidth="1" style="3" min="17" max="17"/>
     <col width="13.7259259259259" customWidth="1" style="3" min="18" max="18"/>
-    <col width="14" customWidth="1" style="3" min="19" max="19"/>
+    <col width="12.5333333333333" customWidth="1" style="3" min="19" max="19"/>
     <col width="4.18518518518519" customWidth="1" style="3" min="20" max="20"/>
     <col width="10.8148148148148" customWidth="1" style="3" min="21" max="21"/>
     <col width="9.81481481481481" customWidth="1" style="3" min="22" max="22"/>
@@ -2322,12 +2322,7 @@
       </c>
       <c r="T2" s="12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> {
-        "select":
-            {
-                # "select_one": "select username,password as pwd  from lea.user where username ='luoshunwen003';"
-            }
-    }</t>
+          <t>{"select":{"select_one": "select username,password as pwd  from lea.user where username ='luoshunwen003';"}}</t>
         </is>
       </c>
       <c r="U2" s="13" t="n"/>
@@ -2555,7 +2550,7 @@
       </c>
       <c r="Z4" s="13" t="inlineStr">
         <is>
-          <t>[{'检查项': '200', '期望值': '200', '实际值': '200', '断言方法': 'eq:实际值与期望值相等', '断言结果': '通过'}, {'检查项': 397.8, '期望值': 300, '实际值': 397.8, '断言方法': 'gte:实际值大于或等于期望值', '断言结果': '通过'}]</t>
+          <t>[{'检查项': '200', '期望值': '200', '实际值': '200', '断言方法': 'eq:实际值与期望值相等', '断言结果': '通过'}, {'检查项': 419.79, '期望值': 300, '实际值': 419.79, '断言方法': 'gte:实际值大于或等于期望值', '断言结果': '通过'}]</t>
         </is>
       </c>
       <c r="AA4" s="5" t="n"/>

</xml_diff>